<commit_message>
coding.html and coffee.html edited------few details added
</commit_message>
<xml_diff>
--- a/microsoft-django-course.xlsx
+++ b/microsoft-django-course.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3192" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3067" uniqueCount="85">
   <si>
     <t>Create data-driven websites by using the Python framework Django</t>
   </si>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="F5" sqref="D5:F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,9 +730,6 @@
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G5" s="1" t="s">
         <v>84</v>
       </c>
@@ -772,9 +769,6 @@
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G6" s="1" t="s">
         <v>84</v>
       </c>
@@ -814,9 +808,6 @@
       <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G7" s="1" t="s">
         <v>84</v>
       </c>
@@ -856,9 +847,6 @@
       <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G8" s="1" t="s">
         <v>84</v>
       </c>
@@ -898,9 +886,6 @@
       <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G9" s="1" t="s">
         <v>84</v>
       </c>
@@ -940,9 +925,6 @@
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G10" s="1" t="s">
         <v>84</v>
       </c>
@@ -982,9 +964,6 @@
       <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G11" s="1" t="s">
         <v>84</v>
       </c>
@@ -1024,9 +1003,6 @@
       <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G12" s="1" t="s">
         <v>84</v>
       </c>
@@ -1066,9 +1042,6 @@
       <c r="E13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G13" s="1" t="s">
         <v>84</v>
       </c>
@@ -1108,9 +1081,6 @@
       <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G14" s="1" t="s">
         <v>84</v>
       </c>
@@ -1148,9 +1118,6 @@
         <v>84</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G15" s="1" t="s">
         <v>84</v>
       </c>
@@ -1190,9 +1157,6 @@
       <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G16" s="1" t="s">
         <v>84</v>
       </c>
@@ -1230,9 +1194,6 @@
         <v>84</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G17" s="1" t="s">
         <v>84</v>
       </c>
@@ -1272,9 +1233,6 @@
       <c r="E18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G18" s="1" t="s">
         <v>84</v>
       </c>
@@ -1314,9 +1272,6 @@
       <c r="E19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G19" s="1" t="s">
         <v>84</v>
       </c>
@@ -1356,9 +1311,6 @@
       <c r="E20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G20" s="1" t="s">
         <v>84</v>
       </c>
@@ -1398,9 +1350,6 @@
       <c r="E21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G21" s="1" t="s">
         <v>84</v>
       </c>
@@ -1440,9 +1389,6 @@
       <c r="E22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G22" s="1" t="s">
         <v>84</v>
       </c>
@@ -1482,9 +1428,6 @@
       <c r="E23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G23" s="1" t="s">
         <v>84</v>
       </c>
@@ -1524,9 +1467,6 @@
       <c r="E24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G24" s="1" t="s">
         <v>84</v>
       </c>
@@ -1566,9 +1506,6 @@
       <c r="E25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G25" s="1" t="s">
         <v>84</v>
       </c>
@@ -1608,9 +1545,6 @@
       <c r="E26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G26" s="1" t="s">
         <v>84</v>
       </c>
@@ -1650,9 +1584,6 @@
       <c r="E27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G27" s="1" t="s">
         <v>84</v>
       </c>
@@ -1692,9 +1623,6 @@
       <c r="E28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G28" s="1" t="s">
         <v>84</v>
       </c>
@@ -1734,9 +1662,6 @@
       <c r="E29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G29" s="1" t="s">
         <v>84</v>
       </c>
@@ -1774,9 +1699,6 @@
         <v>84</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G30" s="1" t="s">
         <v>84</v>
       </c>
@@ -1816,9 +1738,6 @@
       <c r="E31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G31" s="1" t="s">
         <v>84</v>
       </c>
@@ -1858,9 +1777,6 @@
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G32" s="1" t="s">
         <v>84</v>
       </c>
@@ -1900,9 +1816,6 @@
       <c r="E33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G33" s="1" t="s">
         <v>84</v>
       </c>
@@ -1942,9 +1855,6 @@
       <c r="E34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G34" s="1" t="s">
         <v>84</v>
       </c>
@@ -1984,9 +1894,6 @@
       <c r="E35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G35" s="1" t="s">
         <v>84</v>
       </c>
@@ -2024,9 +1931,6 @@
         <v>84</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G36" s="1" t="s">
         <v>84</v>
       </c>
@@ -2064,9 +1968,6 @@
         <v>84</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="F37" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G37" s="1" t="s">
         <v>84</v>
       </c>
@@ -2106,9 +2007,6 @@
       <c r="E38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G38" s="1" t="s">
         <v>84</v>
       </c>
@@ -2148,9 +2046,6 @@
       <c r="E39" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G39" s="1" t="s">
         <v>84</v>
       </c>
@@ -2190,9 +2085,6 @@
       <c r="E40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G40" s="1" t="s">
         <v>84</v>
       </c>
@@ -2232,9 +2124,6 @@
       <c r="E41" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G41" s="1" t="s">
         <v>84</v>
       </c>
@@ -2274,9 +2163,6 @@
       <c r="E42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G42" s="1" t="s">
         <v>84</v>
       </c>
@@ -2316,9 +2202,6 @@
       <c r="E43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G43" s="1" t="s">
         <v>84</v>
       </c>
@@ -2358,9 +2241,6 @@
       <c r="E44" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G44" s="1" t="s">
         <v>84</v>
       </c>
@@ -2400,9 +2280,6 @@
       <c r="E45" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G45" s="1" t="s">
         <v>84</v>
       </c>
@@ -2442,9 +2319,6 @@
       <c r="E46" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G46" s="1" t="s">
         <v>84</v>
       </c>
@@ -2484,9 +2358,6 @@
       <c r="E47" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G47" s="1" t="s">
         <v>84</v>
       </c>
@@ -2524,9 +2395,6 @@
         <v>84</v>
       </c>
       <c r="E48" s="1"/>
-      <c r="F48" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G48" s="1" t="s">
         <v>84</v>
       </c>
@@ -2566,9 +2434,6 @@
       <c r="E49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G49" s="1" t="s">
         <v>84</v>
       </c>
@@ -2608,9 +2473,6 @@
       <c r="E50" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G50" s="1" t="s">
         <v>84</v>
       </c>
@@ -2650,9 +2512,6 @@
       <c r="E51" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G51" s="1" t="s">
         <v>84</v>
       </c>
@@ -2692,9 +2551,6 @@
       <c r="E52" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G52" s="1" t="s">
         <v>84</v>
       </c>
@@ -2734,9 +2590,6 @@
       <c r="E53" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G53" s="1" t="s">
         <v>84</v>
       </c>
@@ -2774,9 +2627,6 @@
         <v>84</v>
       </c>
       <c r="E54" s="1"/>
-      <c r="F54" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G54" s="1" t="s">
         <v>84</v>
       </c>
@@ -2816,9 +2666,6 @@
       <c r="E55" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G55" s="1" t="s">
         <v>84</v>
       </c>
@@ -2858,9 +2705,6 @@
       <c r="E56" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G56" s="1" t="s">
         <v>84</v>
       </c>
@@ -2900,9 +2744,6 @@
       <c r="E57" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G57" s="1" t="s">
         <v>84</v>
       </c>
@@ -2942,9 +2783,6 @@
       <c r="E58" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G58" s="1" t="s">
         <v>84</v>
       </c>
@@ -2984,9 +2822,6 @@
       <c r="E59" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G59" s="1" t="s">
         <v>84</v>
       </c>
@@ -3026,9 +2861,6 @@
       <c r="E60" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G60" s="1" t="s">
         <v>84</v>
       </c>
@@ -3068,9 +2900,6 @@
       <c r="E61" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G61" s="1" t="s">
         <v>84</v>
       </c>
@@ -3110,9 +2939,6 @@
       <c r="E62" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G62" s="1" t="s">
         <v>84</v>
       </c>
@@ -3152,9 +2978,6 @@
       <c r="E63" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G63" s="1" t="s">
         <v>84</v>
       </c>
@@ -3194,9 +3017,6 @@
       <c r="E64" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G64" s="1" t="s">
         <v>84</v>
       </c>
@@ -3236,9 +3056,6 @@
       <c r="E65" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G65" s="1" t="s">
         <v>84</v>
       </c>
@@ -3276,9 +3093,6 @@
         <v>84</v>
       </c>
       <c r="E66" s="1"/>
-      <c r="F66" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G66" s="1" t="s">
         <v>84</v>
       </c>
@@ -3318,9 +3132,6 @@
       <c r="E67" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G67" s="1" t="s">
         <v>84</v>
       </c>
@@ -3360,9 +3171,6 @@
       <c r="E68" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G68" s="1" t="s">
         <v>84</v>
       </c>
@@ -3402,9 +3210,6 @@
       <c r="E69" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G69" s="1" t="s">
         <v>84</v>
       </c>
@@ -3444,9 +3249,6 @@
       <c r="E70" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F70" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G70" s="1" t="s">
         <v>84</v>
       </c>
@@ -3486,9 +3288,6 @@
       <c r="E71" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G71" s="1" t="s">
         <v>84</v>
       </c>
@@ -3526,9 +3325,6 @@
         <v>84</v>
       </c>
       <c r="E72" s="1"/>
-      <c r="F72" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G72" s="1" t="s">
         <v>84</v>
       </c>
@@ -3568,9 +3364,6 @@
       <c r="E73" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G73" s="1" t="s">
         <v>84</v>
       </c>
@@ -3610,9 +3403,6 @@
       <c r="E74" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G74" s="1" t="s">
         <v>84</v>
       </c>
@@ -3652,9 +3442,6 @@
       <c r="E75" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G75" s="1" t="s">
         <v>84</v>
       </c>
@@ -3694,9 +3481,6 @@
       <c r="E76" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G76" s="1" t="s">
         <v>84</v>
       </c>
@@ -3736,9 +3520,6 @@
       <c r="E77" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G77" s="1" t="s">
         <v>84</v>
       </c>
@@ -3778,9 +3559,6 @@
       <c r="E78" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G78" s="1" t="s">
         <v>84</v>
       </c>
@@ -3820,9 +3598,6 @@
       <c r="E79" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G79" s="1" t="s">
         <v>84</v>
       </c>
@@ -3862,9 +3637,6 @@
       <c r="E80" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G80" s="1" t="s">
         <v>84</v>
       </c>
@@ -3904,9 +3676,6 @@
       <c r="E81" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G81" s="1" t="s">
         <v>84</v>
       </c>
@@ -3944,9 +3713,6 @@
         <v>84</v>
       </c>
       <c r="E82" s="1"/>
-      <c r="F82" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G82" s="1" t="s">
         <v>84</v>
       </c>
@@ -3986,9 +3752,6 @@
       <c r="E83" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G83" s="1" t="s">
         <v>84</v>
       </c>
@@ -4028,9 +3791,6 @@
       <c r="E84" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G84" s="1" t="s">
         <v>84</v>
       </c>
@@ -4070,9 +3830,6 @@
       <c r="E85" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G85" s="1" t="s">
         <v>84</v>
       </c>
@@ -4112,9 +3869,6 @@
       <c r="E86" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G86" s="1" t="s">
         <v>84</v>
       </c>
@@ -4154,9 +3908,6 @@
       <c r="E87" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G87" s="1" t="s">
         <v>84</v>
       </c>
@@ -4194,9 +3945,6 @@
         <v>84</v>
       </c>
       <c r="E88" s="1"/>
-      <c r="F88" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G88" s="1" t="s">
         <v>84</v>
       </c>
@@ -4236,9 +3984,6 @@
       <c r="E89" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G89" s="1" t="s">
         <v>84</v>
       </c>
@@ -4278,9 +4023,6 @@
       <c r="E90" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G90" s="1" t="s">
         <v>84</v>
       </c>
@@ -4320,9 +4062,6 @@
       <c r="E91" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G91" s="1" t="s">
         <v>84</v>
       </c>
@@ -4362,9 +4101,6 @@
       <c r="E92" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G92" s="1" t="s">
         <v>84</v>
       </c>
@@ -4404,9 +4140,6 @@
       <c r="E93" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G93" s="1" t="s">
         <v>84</v>
       </c>
@@ -4446,9 +4179,6 @@
       <c r="E94" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G94" s="1" t="s">
         <v>84</v>
       </c>
@@ -4488,9 +4218,6 @@
       <c r="E95" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G95" s="1" t="s">
         <v>84</v>
       </c>
@@ -4530,9 +4257,6 @@
       <c r="E96" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G96" s="1" t="s">
         <v>84</v>
       </c>
@@ -4572,9 +4296,6 @@
       <c r="E97" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G97" s="1" t="s">
         <v>84</v>
       </c>
@@ -4612,9 +4333,6 @@
         <v>84</v>
       </c>
       <c r="E98" s="1"/>
-      <c r="F98" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G98" s="1" t="s">
         <v>84</v>
       </c>
@@ -4654,9 +4372,6 @@
       <c r="E99" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G99" s="1" t="s">
         <v>84</v>
       </c>
@@ -4696,9 +4411,6 @@
       <c r="E100" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F100" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G100" s="1" t="s">
         <v>84</v>
       </c>
@@ -4738,9 +4450,6 @@
       <c r="E101" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F101" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G101" s="1" t="s">
         <v>84</v>
       </c>
@@ -4780,9 +4489,6 @@
       <c r="E102" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F102" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G102" s="1" t="s">
         <v>84</v>
       </c>
@@ -4822,9 +4528,6 @@
       <c r="E103" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F103" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G103" s="1" t="s">
         <v>84</v>
       </c>
@@ -4862,9 +4565,6 @@
         <v>84</v>
       </c>
       <c r="E104" s="1"/>
-      <c r="F104" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G104" s="1" t="s">
         <v>84</v>
       </c>
@@ -4904,9 +4604,6 @@
       <c r="E105" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F105" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G105" s="1" t="s">
         <v>84</v>
       </c>
@@ -4946,9 +4643,6 @@
       <c r="E106" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F106" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G106" s="1" t="s">
         <v>84</v>
       </c>
@@ -4988,9 +4682,6 @@
       <c r="E107" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F107" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G107" s="1" t="s">
         <v>84</v>
       </c>
@@ -5030,9 +4721,6 @@
       <c r="E108" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F108" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G108" s="1" t="s">
         <v>84</v>
       </c>
@@ -5072,9 +4760,6 @@
       <c r="E109" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F109" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G109" s="1" t="s">
         <v>84</v>
       </c>
@@ -5114,9 +4799,6 @@
       <c r="E110" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F110" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G110" s="1" t="s">
         <v>84</v>
       </c>
@@ -5156,9 +4838,6 @@
       <c r="E111" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F111" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G111" s="1" t="s">
         <v>84</v>
       </c>
@@ -5198,9 +4877,6 @@
       <c r="E112" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F112" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G112" s="1" t="s">
         <v>84</v>
       </c>
@@ -5240,9 +4916,6 @@
       <c r="E113" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F113" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G113" s="1" t="s">
         <v>84</v>
       </c>
@@ -5282,9 +4955,6 @@
       <c r="E114" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F114" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G114" s="1" t="s">
         <v>84</v>
       </c>
@@ -5322,9 +4992,6 @@
         <v>84</v>
       </c>
       <c r="E115" s="1"/>
-      <c r="F115" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G115" s="1" t="s">
         <v>84</v>
       </c>
@@ -5364,9 +5031,6 @@
       <c r="E116" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F116" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G116" s="1" t="s">
         <v>84</v>
       </c>
@@ -5406,9 +5070,6 @@
       <c r="E117" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F117" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G117" s="1" t="s">
         <v>84</v>
       </c>
@@ -5448,9 +5109,6 @@
       <c r="E118" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F118" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G118" s="1" t="s">
         <v>84</v>
       </c>
@@ -5490,9 +5148,6 @@
       <c r="E119" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F119" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G119" s="1" t="s">
         <v>84</v>
       </c>
@@ -5532,9 +5187,6 @@
       <c r="E120" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F120" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G120" s="1" t="s">
         <v>84</v>
       </c>
@@ -5572,9 +5224,6 @@
         <v>84</v>
       </c>
       <c r="E121" s="1"/>
-      <c r="F121" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G121" s="1" t="s">
         <v>84</v>
       </c>
@@ -5614,9 +5263,6 @@
       <c r="E122" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F122" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G122" s="1" t="s">
         <v>84</v>
       </c>
@@ -5656,9 +5302,6 @@
       <c r="E123" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F123" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G123" s="1" t="s">
         <v>84</v>
       </c>
@@ -5698,9 +5341,6 @@
       <c r="E124" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F124" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G124" s="1" t="s">
         <v>84</v>
       </c>
@@ -5740,9 +5380,6 @@
       <c r="E125" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F125" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G125" s="1" t="s">
         <v>84</v>
       </c>
@@ -5782,9 +5419,6 @@
       <c r="E126" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F126" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G126" s="1" t="s">
         <v>84</v>
       </c>
@@ -5824,9 +5458,6 @@
       <c r="E127" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F127" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G127" s="1" t="s">
         <v>84</v>
       </c>
@@ -5866,9 +5497,6 @@
       <c r="E128" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F128" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G128" s="1" t="s">
         <v>84</v>
       </c>
@@ -5907,9 +5535,6 @@
       </c>
       <c r="E129" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>84</v>

</xml_diff>